<commit_message>
hasta aqui todo concuerda
</commit_message>
<xml_diff>
--- a/control dinero.xlsx
+++ b/control dinero.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="94">
   <si>
     <t>cantidad</t>
   </si>
@@ -292,13 +292,25 @@
     <t>8 a 14 de junio</t>
   </si>
   <si>
-    <t>medicina</t>
-  </si>
-  <si>
     <t>15 a 21 junio</t>
   </si>
   <si>
-    <t>prestamo, en realidad son 250, pero di 500</t>
+    <t>22 a 28 junio</t>
+  </si>
+  <si>
+    <t>29 junio a 5 de julio</t>
+  </si>
+  <si>
+    <t>ma, luego</t>
+  </si>
+  <si>
+    <t>gym</t>
+  </si>
+  <si>
+    <t>agua</t>
+  </si>
+  <si>
+    <t>1 semana 1 viernes taller</t>
   </si>
 </sst>
 </file>
@@ -409,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -444,15 +456,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -478,10 +489,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A1:F63" totalsRowShown="0">
-  <autoFilter ref="A1:F63"/>
-  <sortState ref="A2:F63">
-    <sortCondition ref="B1:B63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A1:F67" totalsRowShown="0">
+  <autoFilter ref="A1:F67"/>
+  <sortState ref="A2:F67">
+    <sortCondition ref="B1:B67"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="fecha"/>
@@ -797,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X63"/>
+  <dimension ref="A1:X65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,11 +873,11 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
@@ -887,14 +898,14 @@
       </c>
       <c r="G2">
         <f>SUMIFS(Tabla5[cantidad],Tabla5[persona],"ma",Tabla5[pago?],"no")</f>
-        <v>40634</v>
+        <v>40040</v>
       </c>
       <c r="H2">
         <f>SUMIFS(Tabla5[cantidad],Tabla5[persona],"pa",Tabla5[pago?],"no")</f>
-        <v>8789.5</v>
+        <v>7443.5</v>
       </c>
       <c r="I2">
-        <v>634.5</v>
+        <v>3218.5</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
@@ -904,20 +915,20 @@
       </c>
       <c r="L2">
         <f>SUMIFS(Tabla62[cantidad],Tabla62[donde],"tarjeta")</f>
-        <v>2400</v>
+        <v>1761</v>
       </c>
       <c r="M2">
         <f>SUMIFS(Tabla62[cantidad],Tabla62[donde],"fisico")</f>
-        <v>1552.5</v>
+        <v>4850.5</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
@@ -939,7 +950,7 @@
         <v>14</v>
       </c>
       <c r="I3">
-        <v>831</v>
+        <v>558</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -980,7 +991,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>25</v>
@@ -989,10 +1000,10 @@
         <v>7</v>
       </c>
       <c r="L4">
-        <v>2401</v>
+        <v>1763</v>
       </c>
       <c r="M4">
-        <v>1552.5</v>
+        <v>4850.5</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1015,7 +1026,7 @@
         <v>14</v>
       </c>
       <c r="I5">
-        <v>87</v>
+        <v>803</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
@@ -1023,10 +1034,10 @@
       <c r="K5" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="39"/>
+      <c r="M5" s="38"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -1056,7 +1067,7 @@
       </c>
       <c r="L6">
         <f>SUM(L4,-L2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6">
         <f>SUM(M4,-M2)</f>
@@ -1150,26 +1161,26 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="2">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="20">
+        <v>72</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1">
-        <v>677</v>
+        <v>38</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>9</v>
@@ -1179,20 +1190,18 @@
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>88</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2">
-        <v>77</v>
+        <v>619</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>14</v>
@@ -1210,20 +1219,20 @@
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="20">
-        <v>72</v>
+      <c r="A12" s="16"/>
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1"/>
@@ -1241,16 +1250,16 @@
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2">
-        <v>619</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>14</v>
@@ -1270,20 +1279,20 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="8">
-        <v>4</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="20">
+        <v>50</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="1"/>
@@ -1301,38 +1310,47 @@
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="1"/>
+      <c r="I15">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="20">
-        <v>50</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="20" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="11"/>
@@ -1342,19 +1360,20 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="8">
+        <v>35</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="11"/>
@@ -1364,19 +1383,20 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="11"/>
@@ -1387,7 +1407,7 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
@@ -1395,10 +1415,10 @@
         <v>35</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>14</v>
@@ -1409,19 +1429,19 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="20">
         <v>35</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="E20" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="11"/>
@@ -1429,40 +1449,40 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="23">
+      <c r="A21" s="30"/>
+      <c r="B21" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="18">
         <v>35</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="23" t="s">
+      <c r="D21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="11"/>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="18">
-        <v>35</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="19" t="s">
+      <c r="A22" s="30"/>
+      <c r="B22" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="28">
+        <v>150</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="29" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="11"/>
@@ -1472,20 +1492,20 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="18">
-        <v>35</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="19" t="s">
+      <c r="A23" s="27"/>
+      <c r="B23" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="28">
+        <v>84</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="29" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="11"/>
@@ -1495,18 +1515,18 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="28" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="28">
-        <v>150</v>
+        <v>1600</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F24" s="29" t="s">
         <v>14</v>
@@ -1518,20 +1538,20 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="28">
-        <v>84</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="29" t="s">
+      <c r="A25" s="37"/>
+      <c r="B25" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="23">
+        <v>16</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="24" t="s">
         <v>14</v>
       </c>
       <c r="G25" s="15"/>
@@ -1539,18 +1559,18 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="28" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="28">
-        <v>3100</v>
+        <v>11</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F26" s="29" t="s">
         <v>14</v>
@@ -1560,66 +1580,70 @@
       <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="23">
-        <v>16</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="24" t="s">
+      <c r="A27" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="28">
+        <v>250</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="29" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="28">
-        <v>11</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="29" t="s">
+      <c r="A28" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="18">
+        <v>250</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="28">
+      <c r="A29" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="18">
         <v>250</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="28" t="s">
+      <c r="D29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>30</v>
+      <c r="A30" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>29</v>
@@ -1638,68 +1662,68 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="30">
+      <c r="A31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="35">
         <v>250</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="30" t="s">
+      <c r="D31" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="31" t="s">
+      <c r="F31" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="30">
+      <c r="A32" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="35">
         <v>250</v>
       </c>
-      <c r="D32" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="30" t="s">
+      <c r="D32" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="30">
+      <c r="A33" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="35">
         <v>250</v>
       </c>
-      <c r="D33" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="30" t="s">
+      <c r="D33" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
-        <v>47</v>
+      <c r="A34" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>29</v>
@@ -1718,8 +1742,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
-        <v>48</v>
+      <c r="A35" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>29</v>
@@ -1738,8 +1762,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>51</v>
+      <c r="A36" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>29</v>
@@ -1758,48 +1782,48 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="20">
+      <c r="A37" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="8">
         <v>250</v>
       </c>
-      <c r="D37" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="20" t="s">
+      <c r="D37" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="20">
+      <c r="A38" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="8">
         <v>250</v>
       </c>
-      <c r="D38" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="20" t="s">
+      <c r="D38" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
-        <v>59</v>
+      <c r="A39" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>29</v>
@@ -1818,48 +1842,48 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="8">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40">
         <v>250</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" s="8" t="s">
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="8">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41">
         <v>250</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" s="8" t="s">
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
@@ -1879,7 +1903,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
@@ -1899,13 +1923,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
       <c r="C44">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>26</v>
@@ -1919,19 +1943,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
         <v>29</v>
       </c>
       <c r="C45">
-        <v>250</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
         <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -1939,19 +1963,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
         <v>29</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
         <v>26</v>
       </c>
       <c r="E46" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -1959,7 +1983,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B47" t="s">
         <v>29</v>
@@ -1978,8 +2002,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>76</v>
+      <c r="A48" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="B48" t="s">
         <v>29</v>
@@ -1998,8 +2022,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>77</v>
+      <c r="A49" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="B49" t="s">
         <v>29</v>
@@ -2019,119 +2043,119 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50">
+        <v>31</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="2">
+        <v>77.5</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="8">
+        <v>21</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52">
+        <v>66</v>
+      </c>
+      <c r="D52" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53">
+        <v>27</v>
+      </c>
+      <c r="D53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="2">
         <v>77</v>
       </c>
-      <c r="D50" t="s">
-        <v>26</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F50" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51">
+      <c r="F54" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="2">
         <v>77</v>
       </c>
-      <c r="D51" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F51" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" s="2">
-        <v>77.5</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" s="8">
-        <v>21</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54">
-        <v>66</v>
-      </c>
-      <c r="D54" t="s">
-        <v>52</v>
-      </c>
-      <c r="E54" t="s">
-        <v>23</v>
-      </c>
-      <c r="F54" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55">
-        <v>27</v>
-      </c>
-      <c r="D55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>84</v>
+      <c r="A56" s="32" t="s">
+        <v>86</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>29</v>
@@ -2150,8 +2174,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
-        <v>85</v>
+      <c r="A57" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>29</v>
@@ -2170,42 +2194,42 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" s="2">
+      <c r="A58" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58">
         <v>77</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" s="2" t="s">
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C59" s="2">
+      <c r="A59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59">
         <v>77</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="2" t="s">
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F59" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2246,25 +2270,57 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
+      <c r="A62" s="32"/>
       <c r="B62" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C62" s="2">
+        <v>330</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="32"/>
+      <c r="B63" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="2">
-        <v>500</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="C63" s="2">
+        <v>40</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
+      <c r="F63" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="22"/>
+      <c r="B64" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>